<commit_message>
Changes in test file
</commit_message>
<xml_diff>
--- a/Test_model_b.xlsx
+++ b/Test_model_b.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="45">
   <si>
     <t xml:space="preserve">patient_id</t>
   </si>
@@ -31,12 +31,27 @@
     <t xml:space="preserve">P_00032</t>
   </si>
   <si>
+    <t xml:space="preserve">P_00145</t>
+  </si>
+  <si>
     <t xml:space="preserve">P_00343</t>
   </si>
   <si>
+    <t xml:space="preserve">P_00379</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P_00381</t>
+  </si>
+  <si>
     <t xml:space="preserve">P_00409</t>
   </si>
   <si>
+    <t xml:space="preserve">P_00457</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P_00510</t>
+  </si>
+  <si>
     <t xml:space="preserve">P_00641</t>
   </si>
   <si>
@@ -52,7 +67,16 @@
     <t xml:space="preserve">P_01378</t>
   </si>
   <si>
+    <t xml:space="preserve">P_01551</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P_01595</t>
+  </si>
+  <si>
     <t xml:space="preserve">P_01673</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P_01690</t>
   </si>
   <si>
     <t xml:space="preserve">P_01765</t>
@@ -140,7 +164,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -167,12 +191,6 @@
       <sz val="11"/>
       <name val="Cambria"/>
       <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -239,19 +257,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -334,8 +352,8 @@
   </sheetPr>
   <dimension ref="A1:B1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2:B81"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B40" activeCellId="0" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -372,7 +390,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -380,7 +398,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -388,7 +406,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -396,28 +414,28 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" s="2" t="n">
         <v>0</v>
@@ -425,7 +443,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11" s="2" t="n">
         <v>0</v>
@@ -433,7 +451,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12" s="2" t="n">
         <v>0</v>
@@ -441,7 +459,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13" s="2" t="n">
         <v>0</v>
@@ -449,7 +467,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B14" s="2" t="n">
         <v>0</v>
@@ -457,7 +475,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B15" s="2" t="n">
         <v>0</v>
@@ -465,7 +483,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B16" s="2" t="n">
         <v>0</v>
@@ -473,7 +491,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B17" s="2" t="n">
         <v>0</v>
@@ -481,82 +499,82 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B18" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B19" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B20" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B21" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B22" s="2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B23" s="2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B24" s="2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B25" s="2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B26" s="2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B27" s="2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -564,7 +582,7 @@
         <v>14</v>
       </c>
       <c r="B28" s="2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -572,7 +590,7 @@
         <v>14</v>
       </c>
       <c r="B29" s="2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -580,7 +598,7 @@
         <v>15</v>
       </c>
       <c r="B30" s="2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -588,76 +606,76 @@
         <v>15</v>
       </c>
       <c r="B31" s="2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B32" s="2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B33" s="2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B34" s="2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B35" s="2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B36" s="2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B37" s="2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B38" s="2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B39" s="2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B40" s="2" t="n">
         <v>2</v>
@@ -665,7 +683,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B41" s="2" t="n">
         <v>2</v>
@@ -673,7 +691,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B42" s="2" t="n">
         <v>2</v>
@@ -681,7 +699,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B43" s="2" t="n">
         <v>2</v>
@@ -689,7 +707,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B44" s="2" t="n">
         <v>2</v>
@@ -697,7 +715,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B45" s="2" t="n">
         <v>2</v>
@@ -705,7 +723,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B46" s="2" t="n">
         <v>2</v>
@@ -713,7 +731,7 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B47" s="2" t="n">
         <v>2</v>
@@ -721,7 +739,7 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B48" s="2" t="n">
         <v>2</v>
@@ -729,7 +747,7 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B49" s="2" t="n">
         <v>2</v>
@@ -769,7 +787,7 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B54" s="2" t="n">
         <v>2</v>
@@ -777,7 +795,7 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B55" s="2" t="n">
         <v>2</v>
@@ -785,7 +803,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B56" s="2" t="n">
         <v>2</v>
@@ -793,7 +811,7 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B57" s="2" t="n">
         <v>2</v>
@@ -801,7 +819,7 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B58" s="2" t="n">
         <v>2</v>
@@ -809,7 +827,7 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B59" s="2" t="n">
         <v>2</v>
@@ -817,7 +835,7 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B60" s="2" t="n">
         <v>2</v>
@@ -825,7 +843,7 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B61" s="2" t="n">
         <v>2</v>
@@ -849,7 +867,7 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B64" s="2" t="n">
         <v>2</v>
@@ -857,7 +875,7 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B65" s="2" t="n">
         <v>2</v>
@@ -865,7 +883,7 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B66" s="2" t="n">
         <v>2</v>
@@ -873,7 +891,7 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B67" s="2" t="n">
         <v>2</v>
@@ -881,7 +899,7 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B68" s="2" t="n">
         <v>2</v>
@@ -889,7 +907,7 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B69" s="2" t="n">
         <v>2</v>
@@ -897,18 +915,18 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B70" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B71" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -916,7 +934,7 @@
         <v>32</v>
       </c>
       <c r="B72" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -924,7 +942,7 @@
         <v>32</v>
       </c>
       <c r="B73" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -932,7 +950,7 @@
         <v>33</v>
       </c>
       <c r="B74" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -940,7 +958,7 @@
         <v>33</v>
       </c>
       <c r="B75" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -948,7 +966,7 @@
         <v>34</v>
       </c>
       <c r="B76" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -956,7 +974,7 @@
         <v>34</v>
       </c>
       <c r="B77" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -964,7 +982,7 @@
         <v>35</v>
       </c>
       <c r="B78" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -972,7 +990,7 @@
         <v>35</v>
       </c>
       <c r="B79" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -980,7 +998,7 @@
         <v>36</v>
       </c>
       <c r="B80" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -988,80 +1006,152 @@
         <v>36</v>
       </c>
       <c r="B81" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="3"/>
-      <c r="B82" s="4"/>
-    </row>
-    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="3"/>
-      <c r="B83" s="4"/>
-    </row>
-    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="3"/>
-      <c r="B84" s="4"/>
-    </row>
-    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="3"/>
-      <c r="B85" s="4"/>
-    </row>
-    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="3"/>
-      <c r="B86" s="4"/>
-    </row>
-    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="3"/>
-      <c r="B87" s="4"/>
-    </row>
-    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="3"/>
-      <c r="B88" s="4"/>
-    </row>
-    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="3"/>
-      <c r="B89" s="4"/>
-    </row>
-    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="3"/>
-      <c r="B90" s="4"/>
-    </row>
-    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="3"/>
-      <c r="B91" s="4"/>
-    </row>
-    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="3"/>
-      <c r="B92" s="4"/>
-    </row>
-    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="3"/>
-      <c r="B93" s="4"/>
-    </row>
-    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="3"/>
-      <c r="B94" s="4"/>
-    </row>
-    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="3"/>
-      <c r="B95" s="4"/>
-    </row>
-    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="3"/>
-      <c r="B96" s="4"/>
-    </row>
-    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="3"/>
-      <c r="B97" s="4"/>
-    </row>
-    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="3"/>
-      <c r="B98" s="4"/>
-    </row>
-    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="3"/>
-      <c r="B99" s="4"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B82" s="2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B83" s="2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B84" s="2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B85" s="2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B86" s="2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B87" s="2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B88" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B89" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B90" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B91" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B92" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B93" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B94" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B95" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B96" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B97" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B98" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B99" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="3"/>

</xml_diff>